<commit_message>
Fixed parking spot location on Pidkovy st., 1
</commit_message>
<xml_diff>
--- a/parking.xlsx
+++ b/parking.xlsx
@@ -1733,7 +1733,7 @@
     <t xml:space="preserve">Підкови І., пл. </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8410830,24.0293380</t>
+    <t xml:space="preserve">49.8413471,24.0291207</t>
   </si>
   <si>
     <t xml:space="preserve">Галицький р-н, вулиця Підкови І., пл.  1</t>
@@ -2995,11 +2995,11 @@
   </sheetPr>
   <dimension ref="A1:L372"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A295" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F295" activeCellId="0" sqref="F295"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B177" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I223" activeCellId="0" sqref="I223"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.83"/>

</xml_diff>

<commit_message>
added 77 more parking lots
</commit_message>
<xml_diff>
--- a/parking.xlsx
+++ b/parking.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2302" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2302" uniqueCount="957">
   <si>
     <t xml:space="preserve">district</t>
   </si>
@@ -1769,7 +1769,7 @@
     <t xml:space="preserve">Раппапорта Я. </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8452323,24.0202823</t>
+    <t xml:space="preserve">49.8445494,24.0180645</t>
   </si>
   <si>
     <t xml:space="preserve">Шевченківський р-н, вулиця Раппапорта Я.</t>
@@ -1790,13 +1790,13 @@
     <t xml:space="preserve">(згідно з детальним планом території (для обслуговування Палацу спорту))</t>
   </si>
   <si>
-    <t xml:space="preserve">49.8494560,23.9615889</t>
+    <t xml:space="preserve">49.8489040,23.9616470</t>
   </si>
   <si>
     <t xml:space="preserve">Залізничний р-н, вулиця Роксоляни  59</t>
   </si>
   <si>
-    <t xml:space="preserve">49.8460880,23.9594378</t>
+    <t xml:space="preserve">49.8458513,23.9599659</t>
   </si>
   <si>
     <t xml:space="preserve">Залізничний р-н, вулиця Роксоляни  43</t>
@@ -1892,7 +1892,7 @@
     <t xml:space="preserve">Садова </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8209490,23.9879319</t>
+    <t xml:space="preserve">49.8213456,23.9883424</t>
   </si>
   <si>
     <t xml:space="preserve">Залізничний р-н, вулиця Садова  1</t>
@@ -1901,7 +1901,7 @@
     <t xml:space="preserve">Саксаганського П. </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8356724,24.0343672</t>
+    <t xml:space="preserve">49.8345305,24.0330502</t>
   </si>
   <si>
     <t xml:space="preserve">Галицький р-н, вулиця Саксаганського П.</t>
@@ -1910,7 +1910,7 @@
     <t xml:space="preserve">Самчука У. </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8267013,24.0336803</t>
+    <t xml:space="preserve">49.8264736,24.0331941</t>
   </si>
   <si>
     <t xml:space="preserve">Галицький р-н, вулиця Самчука У.</t>
@@ -1922,7 +1922,7 @@
     <t xml:space="preserve"> 58-а</t>
   </si>
   <si>
-    <t xml:space="preserve">49.8261176,24.0116338</t>
+    <t xml:space="preserve">49.8249957,24.0105611</t>
   </si>
   <si>
     <t xml:space="preserve">Франківський р-н, вулиця Сахарова А.,акад.   58-а</t>
@@ -1946,6 +1946,9 @@
     <t xml:space="preserve">Франківський р-н, вулиця Сахарова А.,акад.   19-а</t>
   </si>
   <si>
+    <t xml:space="preserve">49.8209266,24.0174664</t>
+  </si>
+  <si>
     <t xml:space="preserve">49.8235210,24.0176766</t>
   </si>
   <si>
@@ -1955,7 +1958,7 @@
     <t xml:space="preserve">Сахарова А.,акад. – Бойківська </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8225730,24.0175886</t>
+    <t xml:space="preserve">49.8230763,24.0128763</t>
   </si>
   <si>
     <t xml:space="preserve">Франківський р-н, вулиця Сахарова А.,акад. – Бойківська</t>
@@ -1979,7 +1982,7 @@
     <t xml:space="preserve">Святого Теодора, пл. </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8477947,24.0273370</t>
+    <t xml:space="preserve">49.8475352,24.0267888</t>
   </si>
   <si>
     <t xml:space="preserve">Галицький р-н, вулиця Святого Теодора, пл.</t>
@@ -2006,25 +2009,28 @@
     <t xml:space="preserve">Скрипника М. </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8427995,24.0484761</t>
+    <t xml:space="preserve">49.7882453,24.0558302</t>
   </si>
   <si>
     <t xml:space="preserve">Сихівський р-н, вулиця Скрипника М.  9</t>
   </si>
   <si>
-    <t xml:space="preserve">49.8426561,24.0485376</t>
+    <t xml:space="preserve">49.7883349,24.0576821</t>
   </si>
   <si>
     <t xml:space="preserve">Сихівський р-н, вулиця Скрипника М.  1</t>
   </si>
   <si>
+    <t xml:space="preserve">49.7886078,24.0547744</t>
+  </si>
+  <si>
     <t xml:space="preserve">Сихівський р-н, вулиця Скрипника М.  13</t>
   </si>
   <si>
     <t xml:space="preserve">Словацького Ю. </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8389804,24.0252242</t>
+    <t xml:space="preserve">49.8380344,24.0236537</t>
   </si>
   <si>
     <t xml:space="preserve">Галицький р-н, вулиця Словацького Ю.</t>
@@ -2048,7 +2054,7 @@
     <t xml:space="preserve">Солодова </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8418503,24.0492213</t>
+    <t xml:space="preserve">49.8411786,24.0481125</t>
   </si>
   <si>
     <t xml:space="preserve">Личаківський р-н, вулиця Солодова</t>
@@ -2060,7 +2066,7 @@
     <t xml:space="preserve"> 4-б</t>
   </si>
   <si>
-    <t xml:space="preserve">49.8379700,24.0652479</t>
+    <t xml:space="preserve">49.8377030,24.0652233</t>
   </si>
   <si>
     <t xml:space="preserve">Личаківський р-н, вулиця Станція Личаків   4-б</t>
@@ -2084,7 +2090,7 @@
     <t xml:space="preserve">Стефаника В. </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8374008,24.0294859</t>
+    <t xml:space="preserve">49.8362239,24.0267490</t>
   </si>
   <si>
     <t xml:space="preserve">Галицький р-н, вулиця Стефаника В.</t>
@@ -2093,7 +2099,7 @@
     <t xml:space="preserve">Стецька Я. </t>
   </si>
   <si>
-    <t xml:space="preserve">49.8358072,24.0339147</t>
+    <t xml:space="preserve">49.8352270,24.0336068</t>
   </si>
   <si>
     <t xml:space="preserve">Галицький р-н, вулиця Стецька Я.</t>
@@ -2114,7 +2120,7 @@
     <t xml:space="preserve">49.7855265,24.0156913</t>
   </si>
   <si>
-    <t xml:space="preserve">Сихівський р-н, вулиця Стрийська  195</t>
+    <t xml:space="preserve">Сихівський р-н, вулиця Стрийська  195 (Наразі паркінг не облаштовано, скористайтесь наступним)</t>
   </si>
   <si>
     <t xml:space="preserve">49.8192777,24.0194320</t>
@@ -2135,6 +2141,27 @@
     <t xml:space="preserve">Франківський р-н, вулиця Стрийська  144</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Франківський р-н, вулиця Стрийська  104 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Наразі паркінг не облаштовано, скористайтесь наступним)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">49.7881222,24.0175931</t>
   </si>
   <si>
@@ -2150,7 +2177,46 @@
     <t xml:space="preserve">49.7777250,24.0157121</t>
   </si>
   <si>
-    <t xml:space="preserve">Сихівський р-н, вулиця Стрийська  179</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Сихівський р-н, вулиця Стрийська  179 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Наразі паркінг не облаштовано, скористайтесь наступним)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Сихівський р-н, вулиця Стрийська  109 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Наразі паркінг не облаштовано, скористайтесь наступним)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">49.8276211,24.0296910</t>
@@ -2171,7 +2237,25 @@
     <t xml:space="preserve">49.8094836,24.0205319</t>
   </si>
   <si>
-    <t xml:space="preserve">Франківський р-н, вулиця Стрийська - Володимира Великого</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Франківський р-н, вулиця Стрийська - Володимира Великого </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Наразі паркінг не облаштовано, скористайтесь наступним)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Стрілецька </t>
@@ -2893,7 +2977,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2922,6 +3006,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3010,18 +3100,18 @@
   </sheetPr>
   <dimension ref="A1:L372"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B240" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I221" activeCellId="0" sqref="I221"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A257" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A279" activeCellId="0" sqref="A279"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.77"/>
@@ -11083,7 +11173,7 @@
         <v>2</v>
       </c>
       <c r="I246" s="2" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="J246" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D246,  " ", E246, " ", "Львів")</f>
@@ -11116,14 +11206,14 @@
         <v>1</v>
       </c>
       <c r="I247" s="2" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="J247" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D247,  " ", E247, " ", "Львів")</f>
         <v>Сахарова А.,акад.  35 Львів</v>
       </c>
       <c r="K247" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11137,7 +11227,7 @@
         <v>14</v>
       </c>
       <c r="D248" s="0" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E248" s="3"/>
       <c r="G248" s="0" t="n">
@@ -11147,14 +11237,14 @@
         <v>3.5</v>
       </c>
       <c r="I248" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="J248" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D248,  " ", E248, " ", "Львів")</f>
         <v>Сахарова А.,акад. – Бойківська   Львів</v>
       </c>
       <c r="K248" s="0" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11168,7 +11258,7 @@
         <v>14</v>
       </c>
       <c r="D249" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E249" s="3"/>
       <c r="G249" s="0" t="n">
@@ -11178,14 +11268,14 @@
         <v>0</v>
       </c>
       <c r="I249" s="2" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="J249" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D249,  " ", E249, " ", "Львів")</f>
         <v>Свободи, просп.   Львів</v>
       </c>
       <c r="K249" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11199,7 +11289,7 @@
         <v>14</v>
       </c>
       <c r="D250" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E250" s="3" t="n">
         <v>13</v>
@@ -11211,14 +11301,14 @@
         <v>1</v>
       </c>
       <c r="I250" s="2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="J250" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D250,  " ", E250, " ", "Львів")</f>
         <v>Свободи, просп.  13 Львів</v>
       </c>
       <c r="K250" s="0" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11232,7 +11322,7 @@
         <v>14</v>
       </c>
       <c r="D251" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E251" s="3" t="n">
         <v>13</v>
@@ -11244,14 +11334,14 @@
         <v>1</v>
       </c>
       <c r="I251" s="2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="J251" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D251,  " ", E251, " ", "Львів")</f>
         <v>Свободи, просп.  13 Львів</v>
       </c>
       <c r="K251" s="0" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11265,7 +11355,7 @@
         <v>14</v>
       </c>
       <c r="D252" s="0" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="E252" s="3"/>
       <c r="G252" s="0" t="n">
@@ -11275,14 +11365,14 @@
         <v>2.5</v>
       </c>
       <c r="I252" s="2" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="J252" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D252,  " ", E252, " ", "Львів")</f>
         <v>Святого Теодора, пл.   Львів</v>
       </c>
       <c r="K252" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11296,7 +11386,7 @@
         <v>14</v>
       </c>
       <c r="D253" s="0" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E253" s="3" t="n">
         <v>5</v>
@@ -11308,14 +11398,14 @@
         <v>1</v>
       </c>
       <c r="I253" s="2" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="J253" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D253,  " ", E253, " ", "Львів")</f>
         <v>Сихівська  5 Львів</v>
       </c>
       <c r="K253" s="0" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11329,10 +11419,10 @@
         <v>14</v>
       </c>
       <c r="D254" s="0" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E254" s="3" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="G254" s="0" t="n">
         <v>3</v>
@@ -11341,14 +11431,14 @@
         <v>1</v>
       </c>
       <c r="I254" s="2" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="J254" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D254,  " ", E254, " ", "Львів")</f>
         <v>Сихівська   24-б Львів</v>
       </c>
       <c r="K254" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11362,7 +11452,7 @@
         <v>14</v>
       </c>
       <c r="D255" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E255" s="3" t="n">
         <v>9</v>
@@ -11374,14 +11464,14 @@
         <v>3.8</v>
       </c>
       <c r="I255" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="J255" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D255,  " ", E255, " ", "Львів")</f>
         <v>Скрипника М.  9 Львів</v>
       </c>
       <c r="K255" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11395,7 +11485,7 @@
         <v>14</v>
       </c>
       <c r="D256" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E256" s="3" t="n">
         <v>1</v>
@@ -11407,14 +11497,14 @@
         <v>2.5</v>
       </c>
       <c r="I256" s="2" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="J256" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D256,  " ", E256, " ", "Львів")</f>
         <v>Скрипника М.  1 Львів</v>
       </c>
       <c r="K256" s="0" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11428,7 +11518,7 @@
         <v>14</v>
       </c>
       <c r="D257" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E257" s="3" t="n">
         <v>13</v>
@@ -11440,14 +11530,14 @@
         <v>14</v>
       </c>
       <c r="I257" s="2" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="J257" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D257,  " ", E257, " ", "Львів")</f>
         <v>Скрипника М.  13 Львів</v>
       </c>
       <c r="K257" s="0" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11461,7 +11551,7 @@
         <v>14</v>
       </c>
       <c r="D258" s="0" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="E258" s="3"/>
       <c r="G258" s="0" t="n">
@@ -11471,14 +11561,14 @@
         <v>3</v>
       </c>
       <c r="I258" s="2" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="J258" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D258,  " ", E258, " ", "Львів")</f>
         <v>Словацького Ю.   Львів</v>
       </c>
       <c r="K258" s="0" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11492,7 +11582,7 @@
         <v>14</v>
       </c>
       <c r="D259" s="0" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="E259" s="3" t="n">
         <v>13</v>
@@ -11504,14 +11594,14 @@
         <v>1</v>
       </c>
       <c r="I259" s="2" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="J259" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D259,  " ", E259, " ", "Львів")</f>
         <v>Соборна, пл.  13 Львів</v>
       </c>
       <c r="K259" s="0" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11525,7 +11615,7 @@
         <v>14</v>
       </c>
       <c r="D260" s="0" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="E260" s="3" t="n">
         <v>1</v>
@@ -11537,14 +11627,14 @@
         <v>1</v>
       </c>
       <c r="I260" s="2" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="J260" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D260,  " ", E260, " ", "Львів")</f>
         <v>Соборна, пл.  1 Львів</v>
       </c>
       <c r="K260" s="0" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11558,7 +11648,7 @@
         <v>14</v>
       </c>
       <c r="D261" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="E261" s="3"/>
       <c r="G261" s="0" t="n">
@@ -11568,14 +11658,14 @@
         <v>1</v>
       </c>
       <c r="I261" s="2" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="J261" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D261,  " ", E261, " ", "Львів")</f>
         <v>Солодова   Львів</v>
       </c>
       <c r="K261" s="0" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11589,10 +11679,10 @@
         <v>14</v>
       </c>
       <c r="D262" s="0" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="E262" s="3" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="G262" s="0" t="n">
         <v>22</v>
@@ -11601,14 +11691,14 @@
         <v>2.2</v>
       </c>
       <c r="I262" s="2" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="J262" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D262,  " ", E262, " ", "Львів")</f>
         <v>Станція Личаків   4-б Львів</v>
       </c>
       <c r="K262" s="0" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11622,7 +11712,7 @@
         <v>14</v>
       </c>
       <c r="D263" s="0" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E263" s="3"/>
       <c r="G263" s="0" t="n">
@@ -11632,14 +11722,14 @@
         <v>0</v>
       </c>
       <c r="I263" s="2" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="J263" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D263,  " ", E263, " ", "Львів")</f>
         <v>Старий Ринок, пл.   Львів</v>
       </c>
       <c r="K263" s="0" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11653,7 +11743,7 @@
         <v>14</v>
       </c>
       <c r="D264" s="0" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E264" s="3" t="n">
         <v>8</v>
@@ -11665,14 +11755,14 @@
         <v>2.7</v>
       </c>
       <c r="I264" s="2" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="J264" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D264,  " ", E264, " ", "Львів")</f>
         <v>Старий Ринок, пл.  8 Львів</v>
       </c>
       <c r="K264" s="0" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11686,7 +11776,7 @@
         <v>14</v>
       </c>
       <c r="D265" s="0" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="E265" s="3"/>
       <c r="G265" s="0" t="n">
@@ -11696,14 +11786,14 @@
         <v>3.6</v>
       </c>
       <c r="I265" s="2" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="J265" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D265,  " ", E265, " ", "Львів")</f>
         <v>Стефаника В.   Львів</v>
       </c>
       <c r="K265" s="0" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11717,7 +11807,7 @@
         <v>14</v>
       </c>
       <c r="D266" s="0" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="E266" s="3"/>
       <c r="G266" s="0" t="n">
@@ -11727,14 +11817,14 @@
         <v>1.7</v>
       </c>
       <c r="I266" s="2" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="J266" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D266,  " ", E266, " ", "Львів")</f>
         <v>Стецька Я.   Львів</v>
       </c>
       <c r="K266" s="0" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11748,7 +11838,7 @@
         <v>14</v>
       </c>
       <c r="D267" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E267" s="3" t="n">
         <v>33</v>
@@ -11760,14 +11850,14 @@
         <v>1</v>
       </c>
       <c r="I267" s="2" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="J267" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D267,  " ", E267, " ", "Львів")</f>
         <v>Стрийська  33 Львів</v>
       </c>
       <c r="K267" s="0" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11781,13 +11871,13 @@
         <v>14</v>
       </c>
       <c r="D268" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E268" s="3" t="n">
         <v>195</v>
       </c>
       <c r="F268" s="0" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="G268" s="0" t="n">
         <v>295</v>
@@ -11796,14 +11886,14 @@
         <v>29.5</v>
       </c>
       <c r="I268" s="2" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="J268" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D268,  " ", E268, " ", "Львів")</f>
         <v>Стрийська  195 Львів</v>
       </c>
       <c r="K268" s="0" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11817,7 +11907,7 @@
         <v>14</v>
       </c>
       <c r="D269" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E269" s="3" t="n">
         <v>84</v>
@@ -11829,14 +11919,14 @@
         <v>1</v>
       </c>
       <c r="I269" s="2" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="J269" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D269,  " ", E269, " ", "Львів")</f>
         <v>Стрийська  84 Львів</v>
       </c>
       <c r="K269" s="0" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11850,7 +11940,7 @@
         <v>14</v>
       </c>
       <c r="D270" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E270" s="3" t="n">
         <v>104</v>
@@ -11862,14 +11952,14 @@
         <v>2</v>
       </c>
       <c r="I270" s="2" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="J270" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D270,  " ", E270, " ", "Львів")</f>
         <v>Стрийська  104 Львів</v>
       </c>
       <c r="K270" s="0" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11883,7 +11973,7 @@
         <v>14</v>
       </c>
       <c r="D271" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E271" s="3" t="n">
         <v>144</v>
@@ -11895,17 +11985,17 @@
         <v>1</v>
       </c>
       <c r="I271" s="2" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="J271" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D271,  " ", E271, " ", "Львів")</f>
         <v>Стрийська  144 Львів</v>
       </c>
       <c r="K271" s="0" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
         <v>39</v>
       </c>
@@ -11916,7 +12006,7 @@
         <v>14</v>
       </c>
       <c r="D272" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E272" s="3" t="n">
         <v>104</v>
@@ -11928,14 +12018,14 @@
         <v>3.8</v>
       </c>
       <c r="I272" s="2" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="J272" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D272,  " ", E272, " ", "Львів")</f>
         <v>Стрийська  104 Львів</v>
       </c>
       <c r="K272" s="0" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11949,7 +12039,7 @@
         <v>14</v>
       </c>
       <c r="D273" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E273" s="3" t="n">
         <v>109</v>
@@ -11961,14 +12051,14 @@
         <v>1</v>
       </c>
       <c r="I273" s="2" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="J273" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D273,  " ", E273, " ", "Львів")</f>
         <v>Стрийська  109 Львів</v>
       </c>
       <c r="K273" s="0" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11982,7 +12072,7 @@
         <v>14</v>
       </c>
       <c r="D274" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E274" s="3" t="n">
         <v>107</v>
@@ -11994,17 +12084,17 @@
         <v>1</v>
       </c>
       <c r="I274" s="2" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="J274" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D274,  " ", E274, " ", "Львів")</f>
         <v>Стрийська  107 Львів</v>
       </c>
       <c r="K274" s="0" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
         <v>65</v>
       </c>
@@ -12015,7 +12105,7 @@
         <v>14</v>
       </c>
       <c r="D275" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E275" s="3" t="n">
         <v>179</v>
@@ -12027,17 +12117,17 @@
         <v>2</v>
       </c>
       <c r="I275" s="2" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="J275" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D275,  " ", E275, " ", "Львів")</f>
         <v>Стрийська  179 Львів</v>
       </c>
       <c r="K275" s="0" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
         <v>65</v>
       </c>
@@ -12048,7 +12138,7 @@
         <v>14</v>
       </c>
       <c r="D276" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E276" s="3" t="n">
         <v>109</v>
@@ -12060,14 +12150,14 @@
         <v>2.3</v>
       </c>
       <c r="I276" s="2" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="J276" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D276,  " ", E276, " ", "Львів")</f>
         <v>Стрийська  109 Львів</v>
       </c>
       <c r="K276" s="0" t="s">
-        <v>704</v>
+        <v>712</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12081,7 +12171,7 @@
         <v>14</v>
       </c>
       <c r="D277" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E277" s="3" t="n">
         <v>28</v>
@@ -12093,14 +12183,14 @@
         <v>1</v>
       </c>
       <c r="I277" s="2" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
       <c r="J277" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D277,  " ", E277, " ", "Львів")</f>
         <v>Стрийська  28 Львів</v>
       </c>
       <c r="K277" s="0" t="s">
-        <v>710</v>
+        <v>714</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12114,7 +12204,7 @@
         <v>14</v>
       </c>
       <c r="D278" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E278" s="3" t="n">
         <v>332</v>
@@ -12126,17 +12216,17 @@
         <v>3.1</v>
       </c>
       <c r="I278" s="2" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="J278" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D278,  " ", E278, " ", "Львів")</f>
         <v>Стрийська  332 Львів</v>
       </c>
       <c r="K278" s="0" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
         <v>39</v>
       </c>
@@ -12147,7 +12237,7 @@
         <v>14</v>
       </c>
       <c r="D279" s="0" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="E279" s="3"/>
       <c r="G279" s="0" t="n">
@@ -12157,14 +12247,14 @@
         <v>10.4</v>
       </c>
       <c r="I279" s="2" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="J279" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D279,  " ", E279, " ", "Львів")</f>
         <v>Стрийська - Володимира Великого   Львів</v>
       </c>
       <c r="K279" s="0" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12178,7 +12268,7 @@
         <v>14</v>
       </c>
       <c r="D280" s="0" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="E280" s="3" t="n">
         <v>10</v>
@@ -12190,14 +12280,14 @@
         <v>0</v>
       </c>
       <c r="I280" s="2" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="J280" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D280,  " ", E280, " ", "Львів")</f>
         <v>Стрілецька  10 Львів</v>
       </c>
       <c r="K280" s="0" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12211,7 +12301,7 @@
         <v>14</v>
       </c>
       <c r="D281" s="0" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="E281" s="3" t="n">
         <v>2</v>
@@ -12223,14 +12313,14 @@
         <v>1</v>
       </c>
       <c r="I281" s="2" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c r="J281" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D281,  " ", E281, " ", "Львів")</f>
         <v>Стуса В.  2 Львів</v>
       </c>
       <c r="K281" s="0" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12244,11 +12334,11 @@
         <v>14</v>
       </c>
       <c r="D282" s="0" t="s">
-        <v>722</v>
+        <v>726</v>
       </c>
       <c r="E282" s="3"/>
       <c r="F282" s="0" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c r="G282" s="0" t="n">
         <v>52</v>
@@ -12257,14 +12347,14 @@
         <v>5.2</v>
       </c>
       <c r="I282" s="2" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="J282" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D282,  " ", E282, " ", "Львів")</f>
         <v>Стуса В.  Львів</v>
       </c>
       <c r="K282" s="0" t="s">
-        <v>725</v>
+        <v>729</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12278,7 +12368,7 @@
         <v>14</v>
       </c>
       <c r="D283" s="0" t="s">
-        <v>726</v>
+        <v>730</v>
       </c>
       <c r="E283" s="3" t="n">
         <v>13</v>
@@ -12290,14 +12380,14 @@
         <v>4</v>
       </c>
       <c r="I283" s="2" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
       <c r="J283" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D283,  " ", E283, " ", "Львів")</f>
         <v>Суботівська  13 Львів</v>
       </c>
       <c r="K283" s="0" t="s">
-        <v>728</v>
+        <v>732</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12311,7 +12401,7 @@
         <v>14</v>
       </c>
       <c r="D284" s="0" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c r="E284" s="3"/>
       <c r="G284" s="0" t="n">
@@ -12321,14 +12411,14 @@
         <v>1.5</v>
       </c>
       <c r="I284" s="2" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c r="J284" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D284,  " ", E284, " ", "Львів")</f>
         <v>Сянська   Львів</v>
       </c>
       <c r="K284" s="0" t="s">
-        <v>731</v>
+        <v>735</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12342,7 +12432,7 @@
         <v>14</v>
       </c>
       <c r="D285" s="0" t="s">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="E285" s="3"/>
       <c r="G285" s="0" t="n">
@@ -12352,14 +12442,14 @@
         <v>1</v>
       </c>
       <c r="I285" s="2" t="s">
-        <v>733</v>
+        <v>737</v>
       </c>
       <c r="J285" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D285,  " ", E285, " ", "Львів")</f>
         <v>Січових Стрільців   Львів</v>
       </c>
       <c r="K285" s="0" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12373,7 +12463,7 @@
         <v>14</v>
       </c>
       <c r="D286" s="0" t="s">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="E286" s="3" t="n">
         <v>9</v>
@@ -12385,14 +12475,14 @@
         <v>1</v>
       </c>
       <c r="I286" s="2" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="J286" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D286,  " ", E286, " ", "Львів")</f>
         <v>Січових Стрільців  9 Львів</v>
       </c>
       <c r="K286" s="0" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12406,7 +12496,7 @@
         <v>14</v>
       </c>
       <c r="D287" s="0" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="E287" s="3"/>
       <c r="G287" s="0" t="n">
@@ -12416,14 +12506,14 @@
         <v>3</v>
       </c>
       <c r="I287" s="2" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="J287" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D287,  " ", E287, " ", "Львів")</f>
         <v>Театральна   Львів</v>
       </c>
       <c r="K287" s="0" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12437,7 +12527,7 @@
         <v>14</v>
       </c>
       <c r="D288" s="0" t="s">
-        <v>740</v>
+        <v>744</v>
       </c>
       <c r="E288" s="3" t="n">
         <v>42</v>
@@ -12449,14 +12539,14 @@
         <v>3</v>
       </c>
       <c r="I288" s="2" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="J288" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D288,  " ", E288, " ", "Львів")</f>
         <v>Тернопільська  42 Львів</v>
       </c>
       <c r="K288" s="0" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12470,10 +12560,10 @@
         <v>14</v>
       </c>
       <c r="D289" s="0" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="E289" s="3" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c r="G289" s="0" t="n">
         <v>4</v>
@@ -12482,14 +12572,14 @@
         <v>1</v>
       </c>
       <c r="I289" s="2" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="J289" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D289,  " ", E289, " ", "Львів")</f>
         <v>Тершаковців   1-б Львів</v>
       </c>
       <c r="K289" s="0" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12503,7 +12593,7 @@
         <v>14</v>
       </c>
       <c r="D290" s="0" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="E290" s="3" t="n">
         <v>2</v>
@@ -12515,14 +12605,14 @@
         <v>1</v>
       </c>
       <c r="I290" s="2" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="J290" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D290,  " ", E290, " ", "Львів")</f>
         <v>Тершаковців  2 Львів</v>
       </c>
       <c r="K290" s="0" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12536,7 +12626,7 @@
         <v>14</v>
       </c>
       <c r="D291" s="0" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="E291" s="3" t="s">
         <v>538</v>
@@ -12548,14 +12638,14 @@
         <v>1</v>
       </c>
       <c r="I291" s="2" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="J291" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D291,  " ", E291, " ", "Львів")</f>
         <v>Тершаковців   6-а Львів</v>
       </c>
       <c r="K291" s="0" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12569,7 +12659,7 @@
         <v>14</v>
       </c>
       <c r="D292" s="0" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="E292" s="3"/>
       <c r="G292" s="0" t="n">
@@ -12579,14 +12669,14 @@
         <v>1</v>
       </c>
       <c r="I292" s="2" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="J292" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D292,  " ", E292, " ", "Львів")</f>
         <v>Тиктора І.   Львів</v>
       </c>
       <c r="K292" s="0" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12600,7 +12690,7 @@
         <v>14</v>
       </c>
       <c r="D293" s="0" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="E293" s="3"/>
       <c r="G293" s="0" t="n">
@@ -12610,14 +12700,14 @@
         <v>2</v>
       </c>
       <c r="I293" s="2" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
       <c r="J293" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D293,  " ", E293, " ", "Львів")</f>
         <v>Тобілевича І.   Львів</v>
       </c>
       <c r="K293" s="0" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12631,7 +12721,7 @@
         <v>14</v>
       </c>
       <c r="D294" s="0" t="s">
-        <v>757</v>
+        <v>761</v>
       </c>
       <c r="E294" s="3"/>
       <c r="G294" s="0" t="n">
@@ -12641,14 +12731,14 @@
         <v>1</v>
       </c>
       <c r="I294" s="2" t="s">
-        <v>758</v>
+        <v>762</v>
       </c>
       <c r="J294" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D294,  " ", E294, " ", "Львів")</f>
         <v>Томашівського С.   Львів</v>
       </c>
       <c r="K294" s="0" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12662,7 +12752,7 @@
         <v>14</v>
       </c>
       <c r="D295" s="0" t="s">
-        <v>760</v>
+        <v>764</v>
       </c>
       <c r="E295" s="3" t="n">
         <v>4</v>
@@ -12674,14 +12764,14 @@
         <v>3</v>
       </c>
       <c r="I295" s="2" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
       <c r="J295" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D295,  " ", E295, " ", "Львів")</f>
         <v>Торф’яна  4 Львів</v>
       </c>
       <c r="K295" s="0" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12695,7 +12785,7 @@
         <v>14</v>
       </c>
       <c r="D296" s="0" t="s">
-        <v>760</v>
+        <v>764</v>
       </c>
       <c r="E296" s="3" t="n">
         <v>25</v>
@@ -12707,14 +12797,14 @@
         <v>2</v>
       </c>
       <c r="I296" s="2" t="s">
-        <v>763</v>
+        <v>767</v>
       </c>
       <c r="J296" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D296,  " ", E296, " ", "Львів")</f>
         <v>Торф’яна  25 Львів</v>
       </c>
       <c r="K296" s="0" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12728,7 +12818,7 @@
         <v>14</v>
       </c>
       <c r="D297" s="0" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="E297" s="3" t="n">
         <v>141</v>
@@ -12740,14 +12830,14 @@
         <v>5</v>
       </c>
       <c r="I297" s="2" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
       <c r="J297" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D297,  " ", E297, " ", "Львів")</f>
         <v>Глинянський Тракт  141 Львів</v>
       </c>
       <c r="K297" s="0" t="s">
-        <v>767</v>
+        <v>771</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12761,7 +12851,7 @@
         <v>14</v>
       </c>
       <c r="D298" s="0" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
       <c r="E298" s="3" t="n">
         <v>33</v>
@@ -12773,14 +12863,14 @@
         <v>3</v>
       </c>
       <c r="I298" s="2" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="J298" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D298,  " ", E298, " ", "Львів")</f>
         <v>Трильовського К.  33 Львів</v>
       </c>
       <c r="K298" s="0" t="s">
-        <v>770</v>
+        <v>774</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12794,7 +12884,7 @@
         <v>14</v>
       </c>
       <c r="D299" s="0" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="E299" s="3" t="n">
         <v>25</v>
@@ -12806,14 +12896,14 @@
         <v>1</v>
       </c>
       <c r="I299" s="2" t="s">
-        <v>772</v>
+        <v>776</v>
       </c>
       <c r="J299" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D299,  " ", E299, " ", "Львів")</f>
         <v>Федьковича Ю.  25 Львів</v>
       </c>
       <c r="K299" s="0" t="s">
-        <v>773</v>
+        <v>777</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12827,7 +12917,7 @@
         <v>14</v>
       </c>
       <c r="D300" s="0" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="E300" s="3"/>
       <c r="G300" s="0" t="n">
@@ -12837,14 +12927,14 @@
         <v>5</v>
       </c>
       <c r="I300" s="2" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="J300" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D300,  " ", E300, " ", "Львів")</f>
         <v>Федьковича Ю.   Львів</v>
       </c>
       <c r="K300" s="0" t="s">
-        <v>775</v>
+        <v>779</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12858,7 +12948,7 @@
         <v>14</v>
       </c>
       <c r="D301" s="0" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="E301" s="3" t="n">
         <v>23</v>
@@ -12870,14 +12960,14 @@
         <v>1</v>
       </c>
       <c r="I301" s="2" t="s">
-        <v>777</v>
+        <v>781</v>
       </c>
       <c r="J301" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D301,  " ", E301, " ", "Львів")</f>
         <v>Франка І.  23 Львів</v>
       </c>
       <c r="K301" s="0" t="s">
-        <v>778</v>
+        <v>782</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12891,10 +12981,10 @@
         <v>14</v>
       </c>
       <c r="D302" s="0" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="E302" s="3" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="G302" s="0" t="n">
         <v>15</v>
@@ -12903,14 +12993,14 @@
         <v>2</v>
       </c>
       <c r="I302" s="2" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="J302" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D302,  " ", E302, " ", "Львів")</f>
         <v>Франка І.   101-115 Львів</v>
       </c>
       <c r="K302" s="0" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12924,7 +13014,7 @@
         <v>14</v>
       </c>
       <c r="D303" s="0" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="E303" s="3" t="n">
         <v>66</v>
@@ -12936,14 +13026,14 @@
         <v>1</v>
       </c>
       <c r="I303" s="2" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c r="J303" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D303,  " ", E303, " ", "Львів")</f>
         <v>Франка І.  66 Львів</v>
       </c>
       <c r="K303" s="0" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12957,10 +13047,10 @@
         <v>14</v>
       </c>
       <c r="D304" s="0" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="E304" s="3" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
       <c r="G304" s="0" t="n">
         <v>12</v>
@@ -12969,14 +13059,14 @@
         <v>1</v>
       </c>
       <c r="I304" s="2" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c r="J304" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D304,  " ", E304, " ", "Львів")</f>
         <v>Франка І.   137-а Львів</v>
       </c>
       <c r="K304" s="0" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12990,10 +13080,10 @@
         <v>14</v>
       </c>
       <c r="D305" s="0" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="E305" s="3" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="G305" s="0" t="n">
         <v>2</v>
@@ -13002,14 +13092,14 @@
         <v>1</v>
       </c>
       <c r="I305" s="2" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="J305" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D305,  " ", E305, " ", "Львів")</f>
         <v>Франка І.   75-77 Львів</v>
       </c>
       <c r="K305" s="0" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13023,7 +13113,7 @@
         <v>14</v>
       </c>
       <c r="D306" s="0" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="E306" s="3" t="n">
         <v>108</v>
@@ -13035,14 +13125,14 @@
         <v>1</v>
       </c>
       <c r="I306" s="2" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="J306" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D306,  " ", E306, " ", "Львів")</f>
         <v>Франка І.  108 Львів</v>
       </c>
       <c r="K306" s="0" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13056,7 +13146,7 @@
         <v>14</v>
       </c>
       <c r="D307" s="0" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="E307" s="3"/>
       <c r="G307" s="0" t="n">
@@ -13066,14 +13156,14 @@
         <v>1</v>
       </c>
       <c r="I307" s="2" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="J307" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D307,  " ", E307, " ", "Львів")</f>
         <v>Фредра О.   Львів</v>
       </c>
       <c r="K307" s="0" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13087,7 +13177,7 @@
         <v>14</v>
       </c>
       <c r="D308" s="0" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="E308" s="3" t="n">
         <v>14</v>
@@ -13099,14 +13189,14 @@
         <v>1</v>
       </c>
       <c r="I308" s="2" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
       <c r="J308" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D308,  " ", E308, " ", "Львів")</f>
         <v>Фурманська  14 Львів</v>
       </c>
       <c r="K308" s="0" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13120,7 +13210,7 @@
         <v>14</v>
       </c>
       <c r="D309" s="0" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="E309" s="3" t="n">
         <v>9</v>
@@ -13132,14 +13222,14 @@
         <v>1</v>
       </c>
       <c r="I309" s="2" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="J309" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D309,  " ", E309, " ", "Львів")</f>
         <v>Фурманська  9 Львів</v>
       </c>
       <c r="K309" s="0" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13153,7 +13243,7 @@
         <v>14</v>
       </c>
       <c r="D310" s="0" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="E310" s="3" t="n">
         <v>1</v>
@@ -13165,14 +13255,14 @@
         <v>1</v>
       </c>
       <c r="I310" s="2" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="J310" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D310,  " ", E310, " ", "Львів")</f>
         <v>Фурманська  1 Львів</v>
       </c>
       <c r="K310" s="0" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13186,7 +13276,7 @@
         <v>14</v>
       </c>
       <c r="D311" s="0" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="E311" s="3" t="n">
         <v>4</v>
@@ -13198,14 +13288,14 @@
         <v>2</v>
       </c>
       <c r="I311" s="2" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="J311" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D311,  " ", E311, " ", "Львів")</f>
         <v>Хлібна  4 Львів</v>
       </c>
       <c r="K311" s="0" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13219,7 +13309,7 @@
         <v>14</v>
       </c>
       <c r="D312" s="0" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="E312" s="3" t="n">
         <v>4</v>
@@ -13231,14 +13321,14 @@
         <v>4</v>
       </c>
       <c r="I312" s="2" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="J312" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D312,  " ", E312, " ", "Львів")</f>
         <v>Хлібна  4 Львів</v>
       </c>
       <c r="K312" s="0" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13252,10 +13342,10 @@
         <v>14</v>
       </c>
       <c r="D313" s="0" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="E313" s="3" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c r="G313" s="0" t="n">
         <v>8</v>
@@ -13264,14 +13354,14 @@
         <v>1</v>
       </c>
       <c r="I313" s="2" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c r="J313" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D313,  " ", E313, " ", "Львів")</f>
         <v>Хмельницького Б   216-222 Львів</v>
       </c>
       <c r="K313" s="0" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13285,7 +13375,7 @@
         <v>14</v>
       </c>
       <c r="D314" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E314" s="3" t="n">
         <v>271</v>
@@ -13297,14 +13387,14 @@
         <v>4</v>
       </c>
       <c r="I314" s="2" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
       <c r="J314" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D314,  " ", E314, " ", "Львів")</f>
         <v>Хмельницького Б.  271 Львів</v>
       </c>
       <c r="K314" s="0" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13318,7 +13408,7 @@
         <v>14</v>
       </c>
       <c r="D315" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E315" s="3" t="n">
         <v>271</v>
@@ -13330,14 +13420,14 @@
         <v>1</v>
       </c>
       <c r="I315" s="2" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
       <c r="J315" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D315,  " ", E315, " ", "Львів")</f>
         <v>Хмельницького Б.  271 Львів</v>
       </c>
       <c r="K315" s="0" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13351,7 +13441,7 @@
         <v>14</v>
       </c>
       <c r="D316" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E316" s="3" t="n">
         <v>200</v>
@@ -13363,14 +13453,14 @@
         <v>1</v>
       </c>
       <c r="I316" s="2" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="J316" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D316,  " ", E316, " ", "Львів")</f>
         <v>Хмельницького Б.  200 Львів</v>
       </c>
       <c r="K316" s="0" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13384,7 +13474,7 @@
         <v>14</v>
       </c>
       <c r="D317" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E317" s="3" t="n">
         <v>54</v>
@@ -13396,14 +13486,14 @@
         <v>1</v>
       </c>
       <c r="I317" s="2" t="s">
-        <v>814</v>
+        <v>818</v>
       </c>
       <c r="J317" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D317,  " ", E317, " ", "Львів")</f>
         <v>Хмельницького Б.  54 Львів</v>
       </c>
       <c r="K317" s="0" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13417,10 +13507,10 @@
         <v>14</v>
       </c>
       <c r="D318" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E318" s="3" t="s">
-        <v>816</v>
+        <v>820</v>
       </c>
       <c r="G318" s="0" t="n">
         <v>57</v>
@@ -13429,14 +13519,14 @@
         <v>6</v>
       </c>
       <c r="I318" s="2" t="s">
-        <v>817</v>
+        <v>821</v>
       </c>
       <c r="J318" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D318,  " ", E318, " ", "Львів")</f>
         <v>Хмельницького Б.   188-а Львів</v>
       </c>
       <c r="K318" s="0" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13450,7 +13540,7 @@
         <v>14</v>
       </c>
       <c r="D319" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E319" s="3" t="n">
         <v>106</v>
@@ -13462,14 +13552,14 @@
         <v>1</v>
       </c>
       <c r="I319" s="2" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
       <c r="J319" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D319,  " ", E319, " ", "Львів")</f>
         <v>Хмельницького Б.  106 Львів</v>
       </c>
       <c r="K319" s="0" t="s">
-        <v>820</v>
+        <v>824</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13483,7 +13573,7 @@
         <v>14</v>
       </c>
       <c r="D320" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E320" s="3" t="n">
         <v>172</v>
@@ -13495,14 +13585,14 @@
         <v>1</v>
       </c>
       <c r="I320" s="2" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c r="J320" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D320,  " ", E320, " ", "Львів")</f>
         <v>Хмельницького Б.  172 Львів</v>
       </c>
       <c r="K320" s="0" t="s">
-        <v>822</v>
+        <v>826</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13516,7 +13606,7 @@
         <v>14</v>
       </c>
       <c r="D321" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E321" s="3" t="n">
         <v>212</v>
@@ -13528,14 +13618,14 @@
         <v>11</v>
       </c>
       <c r="I321" s="2" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
       <c r="J321" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D321,  " ", E321, " ", "Львів")</f>
         <v>Хмельницького Б.  212 Львів</v>
       </c>
       <c r="K321" s="0" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13549,7 +13639,7 @@
         <v>14</v>
       </c>
       <c r="D322" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E322" s="3" t="n">
         <v>230</v>
@@ -13561,14 +13651,14 @@
         <v>5</v>
       </c>
       <c r="I322" s="2" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="J322" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D322,  " ", E322, " ", "Львів")</f>
         <v>Хмельницького Б.  230 Львів</v>
       </c>
       <c r="K322" s="0" t="s">
-        <v>826</v>
+        <v>830</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13582,13 +13672,13 @@
         <v>14</v>
       </c>
       <c r="D323" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E323" s="3" t="n">
         <v>83</v>
       </c>
       <c r="F323" s="0" t="s">
-        <v>827</v>
+        <v>831</v>
       </c>
       <c r="G323" s="0" t="n">
         <v>3</v>
@@ -13597,14 +13687,14 @@
         <v>1</v>
       </c>
       <c r="I323" s="2" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
       <c r="J323" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D323,  " ", E323, " ", "Львів")</f>
         <v>Хмельницького Б.  83 Львів</v>
       </c>
       <c r="K323" s="0" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13618,7 +13708,7 @@
         <v>14</v>
       </c>
       <c r="D324" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="E324" s="3" t="n">
         <v>52</v>
@@ -13630,14 +13720,14 @@
         <v>2</v>
       </c>
       <c r="I324" s="2" t="s">
-        <v>831</v>
+        <v>835</v>
       </c>
       <c r="J324" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D324,  " ", E324, " ", "Львів")</f>
         <v>Хоткевича Г.  52 Львів</v>
       </c>
       <c r="K324" s="0" t="s">
-        <v>832</v>
+        <v>836</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13651,7 +13741,7 @@
         <v>14</v>
       </c>
       <c r="D325" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="E325" s="3" t="n">
         <v>10</v>
@@ -13663,14 +13753,14 @@
         <v>3</v>
       </c>
       <c r="I325" s="2" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c r="J325" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D325,  " ", E325, " ", "Львів")</f>
         <v>Хоткевича Г.  10 Львів</v>
       </c>
       <c r="K325" s="0" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13684,7 +13774,7 @@
         <v>14</v>
       </c>
       <c r="D326" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="E326" s="3" t="n">
         <v>64</v>
@@ -13696,14 +13786,14 @@
         <v>9</v>
       </c>
       <c r="I326" s="2" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="J326" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D326,  " ", E326, " ", "Львів")</f>
         <v>Хоткевича Г.  64 Львів</v>
       </c>
       <c r="K326" s="0" t="s">
-        <v>836</v>
+        <v>840</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13717,11 +13807,11 @@
         <v>14</v>
       </c>
       <c r="D327" s="0" t="s">
-        <v>837</v>
+        <v>841</v>
       </c>
       <c r="E327" s="3"/>
       <c r="F327" s="0" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="G327" s="0" t="n">
         <v>4</v>
@@ -13730,14 +13820,14 @@
         <v>1</v>
       </c>
       <c r="I327" s="2" t="s">
-        <v>839</v>
+        <v>843</v>
       </c>
       <c r="J327" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D327,  " ", E327, " ", "Львів")</f>
         <v>Хоткевича Г.  Львів</v>
       </c>
       <c r="K327" s="0" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13751,10 +13841,10 @@
         <v>14</v>
       </c>
       <c r="D328" s="0" t="s">
-        <v>841</v>
+        <v>845</v>
       </c>
       <c r="E328" s="3" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
       <c r="G328" s="0" t="n">
         <v>38</v>
@@ -13763,14 +13853,14 @@
         <v>4</v>
       </c>
       <c r="I328" s="2" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="J328" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D328,  " ", E328, " ", "Львів")</f>
         <v>Хуторівка   40-а Львів</v>
       </c>
       <c r="K328" s="0" t="s">
-        <v>844</v>
+        <v>848</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13784,7 +13874,7 @@
         <v>14</v>
       </c>
       <c r="D329" s="0" t="s">
-        <v>845</v>
+        <v>849</v>
       </c>
       <c r="E329" s="3"/>
       <c r="G329" s="0" t="n">
@@ -13794,14 +13884,14 @@
         <v>2</v>
       </c>
       <c r="I329" s="2" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c r="J329" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D329,  " ", E329, " ", "Львів")</f>
         <v>Хуторівка - Г.Хоткевича   Львів</v>
       </c>
       <c r="K329" s="0" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13812,11 +13902,11 @@
         <v>24</v>
       </c>
       <c r="D330" s="0" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="E330" s="3"/>
       <c r="F330" s="0" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="G330" s="0" t="n">
         <v>238</v>
@@ -13825,14 +13915,14 @@
         <v>24</v>
       </c>
       <c r="I330" s="2" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="J330" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D330,  " ", E330, " ", "Львів")</f>
         <v>ЦА Аеропорт  Львів</v>
       </c>
       <c r="K330" s="0" t="s">
-        <v>851</v>
+        <v>855</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13846,7 +13936,7 @@
         <v>14</v>
       </c>
       <c r="D331" s="0" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="E331" s="3" t="n">
         <v>3</v>
@@ -13858,14 +13948,14 @@
         <v>1</v>
       </c>
       <c r="I331" s="2" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="J331" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D331,  " ", E331, " ", "Львів")</f>
         <v>Цехова  3 Львів</v>
       </c>
       <c r="K331" s="0" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13879,7 +13969,7 @@
         <v>14</v>
       </c>
       <c r="D332" s="0" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c r="E332" s="3"/>
       <c r="G332" s="0" t="n">
@@ -13889,14 +13979,14 @@
         <v>4</v>
       </c>
       <c r="I332" s="2" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="J332" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D332,  " ", E332, " ", "Львів")</f>
         <v>Чайковського П.   Львів</v>
       </c>
       <c r="K332" s="0" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13907,10 +13997,10 @@
         <v>24</v>
       </c>
       <c r="C333" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D333" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E333" s="3" t="n">
         <v>94</v>
@@ -13922,14 +14012,14 @@
         <v>2</v>
       </c>
       <c r="I333" s="2" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="J333" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D333,  " ", E333, " ", "Львів")</f>
         <v>Червоної Калини, просп.  94 Львів</v>
       </c>
       <c r="K333" s="0" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13940,10 +14030,10 @@
         <v>13</v>
       </c>
       <c r="C334" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D334" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E334" s="3" t="n">
         <v>121</v>
@@ -13955,14 +14045,14 @@
         <v>1</v>
       </c>
       <c r="I334" s="2" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="J334" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D334,  " ", E334, " ", "Львів")</f>
         <v>Червоної Калини, просп.  121 Львів</v>
       </c>
       <c r="K334" s="0" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13973,10 +14063,10 @@
         <v>13</v>
       </c>
       <c r="C335" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D335" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E335" s="3" t="n">
         <v>109</v>
@@ -13988,14 +14078,14 @@
         <v>1</v>
       </c>
       <c r="I335" s="2" t="s">
-        <v>864</v>
+        <v>868</v>
       </c>
       <c r="J335" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D335,  " ", E335, " ", "Львів")</f>
         <v>Червоної Калини, просп.  109 Львів</v>
       </c>
       <c r="K335" s="0" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14006,10 +14096,10 @@
         <v>24</v>
       </c>
       <c r="C336" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D336" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E336" s="3" t="n">
         <v>77</v>
@@ -14021,14 +14111,14 @@
         <v>5</v>
       </c>
       <c r="I336" s="2" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="J336" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D336,  " ", E336, " ", "Львів")</f>
         <v>Червоної Калини, просп.  77 Львів</v>
       </c>
       <c r="K336" s="0" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14039,10 +14129,10 @@
         <v>13</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D337" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E337" s="3" t="n">
         <v>77</v>
@@ -14054,14 +14144,14 @@
         <v>1</v>
       </c>
       <c r="I337" s="2" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="J337" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D337,  " ", E337, " ", "Львів")</f>
         <v>Червоної Калини, просп.  77 Львів</v>
       </c>
       <c r="K337" s="0" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14072,10 +14162,10 @@
         <v>13</v>
       </c>
       <c r="C338" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D338" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E338" s="3" t="n">
         <v>40</v>
@@ -14087,14 +14177,14 @@
         <v>1</v>
       </c>
       <c r="I338" s="2" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="J338" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D338,  " ", E338, " ", "Львів")</f>
         <v>Червоної Калини, просп.  40 Львів</v>
       </c>
       <c r="K338" s="0" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14105,10 +14195,10 @@
         <v>13</v>
       </c>
       <c r="C339" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D339" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E339" s="3" t="n">
         <v>35</v>
@@ -14120,14 +14210,14 @@
         <v>1</v>
       </c>
       <c r="I339" s="2" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="J339" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D339,  " ", E339, " ", "Львів")</f>
         <v>Червоної Калини, просп.  35 Львів</v>
       </c>
       <c r="K339" s="0" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14138,10 +14228,10 @@
         <v>40</v>
       </c>
       <c r="C340" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D340" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E340" s="3" t="n">
         <v>94</v>
@@ -14153,14 +14243,14 @@
         <v>1</v>
       </c>
       <c r="I340" s="2" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="J340" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D340,  " ", E340, " ", "Львів")</f>
         <v>Червоної Калини, просп.  94 Львів</v>
       </c>
       <c r="K340" s="0" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14171,13 +14261,13 @@
         <v>24</v>
       </c>
       <c r="C341" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D341" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E341" s="3" t="s">
-        <v>872</v>
+        <v>876</v>
       </c>
       <c r="G341" s="0" t="n">
         <v>38</v>
@@ -14186,14 +14276,14 @@
         <v>4</v>
       </c>
       <c r="I341" s="2" t="s">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c r="J341" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D341,  " ", E341, " ", "Львів")</f>
         <v>Червоної Калини, просп.   68-б Львів</v>
       </c>
       <c r="K341" s="0" t="s">
-        <v>874</v>
+        <v>878</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14204,10 +14294,10 @@
         <v>40</v>
       </c>
       <c r="C342" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D342" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E342" s="3" t="n">
         <v>91</v>
@@ -14219,14 +14309,14 @@
         <v>1</v>
       </c>
       <c r="I342" s="2" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="J342" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D342,  " ", E342, " ", "Львів")</f>
         <v>Червоної Калини, просп.  91 Львів</v>
       </c>
       <c r="K342" s="0" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14237,10 +14327,10 @@
         <v>24</v>
       </c>
       <c r="C343" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D343" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E343" s="3" t="n">
         <v>36</v>
@@ -14252,14 +14342,14 @@
         <v>3</v>
       </c>
       <c r="I343" s="2" t="s">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="J343" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D343,  " ", E343, " ", "Львів")</f>
         <v>Червоної Калини, просп.  36 Львів</v>
       </c>
       <c r="K343" s="0" t="s">
-        <v>878</v>
+        <v>882</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14270,10 +14360,10 @@
         <v>40</v>
       </c>
       <c r="C344" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D344" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="E344" s="3" t="n">
         <v>18</v>
@@ -14285,14 +14375,14 @@
         <v>1</v>
       </c>
       <c r="I344" s="2" t="s">
-        <v>879</v>
+        <v>883</v>
       </c>
       <c r="J344" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D344,  " ", E344, " ", "Львів")</f>
         <v>Червоної Калини, просп.  18 Львів</v>
       </c>
       <c r="K344" s="0" t="s">
-        <v>880</v>
+        <v>884</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14303,10 +14393,10 @@
         <v>24</v>
       </c>
       <c r="C345" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D345" s="0" t="s">
-        <v>881</v>
+        <v>885</v>
       </c>
       <c r="E345" s="3"/>
       <c r="F345" s="0" t="s">
@@ -14319,14 +14409,14 @@
         <v>80</v>
       </c>
       <c r="I345" s="2" t="s">
-        <v>882</v>
+        <v>886</v>
       </c>
       <c r="J345" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D345,  " ", E345, " ", "Львів")</f>
         <v>Червоної Калини, просп. – Скрипника М.  Львів</v>
       </c>
       <c r="K345" s="0" t="s">
-        <v>883</v>
+        <v>887</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14340,7 +14430,7 @@
         <v>14</v>
       </c>
       <c r="D346" s="0" t="s">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="E346" s="3" t="n">
         <v>1</v>
@@ -14352,14 +14442,14 @@
         <v>0</v>
       </c>
       <c r="I346" s="2" t="s">
-        <v>885</v>
+        <v>889</v>
       </c>
       <c r="J346" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D346,  " ", E346, " ", "Львів")</f>
         <v>Чернеча Гора  1 Львів</v>
       </c>
       <c r="K346" s="0" t="s">
-        <v>886</v>
+        <v>890</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14373,7 +14463,7 @@
         <v>14</v>
       </c>
       <c r="D347" s="0" t="s">
-        <v>887</v>
+        <v>891</v>
       </c>
       <c r="E347" s="3" t="n">
         <v>31</v>
@@ -14385,14 +14475,14 @@
         <v>3</v>
       </c>
       <c r="I347" s="2" t="s">
-        <v>888</v>
+        <v>892</v>
       </c>
       <c r="J347" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D347,  " ", E347, " ", "Львів")</f>
         <v>Чигиринська  31 Львів</v>
       </c>
       <c r="K347" s="0" t="s">
-        <v>889</v>
+        <v>893</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14403,10 +14493,10 @@
         <v>13</v>
       </c>
       <c r="C348" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D348" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="E348" s="3" t="n">
         <v>105</v>
@@ -14418,14 +14508,14 @@
         <v>1</v>
       </c>
       <c r="I348" s="2" t="s">
-        <v>891</v>
+        <v>895</v>
       </c>
       <c r="J348" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D348,  " ", E348, " ", "Львів")</f>
         <v>Чорновола В.,просп.  105 Львів</v>
       </c>
       <c r="K348" s="0" t="s">
-        <v>892</v>
+        <v>896</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14436,10 +14526,10 @@
         <v>13</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D349" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="E349" s="3" t="n">
         <v>101</v>
@@ -14451,14 +14541,14 @@
         <v>1</v>
       </c>
       <c r="I349" s="2" t="s">
-        <v>893</v>
+        <v>897</v>
       </c>
       <c r="J349" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D349,  " ", E349, " ", "Львів")</f>
         <v>Чорновола В.,просп.  101 Львів</v>
       </c>
       <c r="K349" s="0" t="s">
-        <v>894</v>
+        <v>898</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14469,10 +14559,10 @@
         <v>13</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D350" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="E350" s="3" t="n">
         <v>95</v>
@@ -14484,14 +14574,14 @@
         <v>1</v>
       </c>
       <c r="I350" s="2" t="s">
-        <v>895</v>
+        <v>899</v>
       </c>
       <c r="J350" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D350,  " ", E350, " ", "Львів")</f>
         <v>Чорновола В.,просп.  95 Львів</v>
       </c>
       <c r="K350" s="0" t="s">
-        <v>896</v>
+        <v>900</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14502,10 +14592,10 @@
         <v>13</v>
       </c>
       <c r="C351" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D351" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="E351" s="3" t="n">
         <v>61</v>
@@ -14517,14 +14607,14 @@
         <v>1</v>
       </c>
       <c r="I351" s="2" t="s">
-        <v>897</v>
+        <v>901</v>
       </c>
       <c r="J351" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D351,  " ", E351, " ", "Львів")</f>
         <v>Чорновола В.,просп.  61 Львів</v>
       </c>
       <c r="K351" s="0" t="s">
-        <v>898</v>
+        <v>902</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14535,10 +14625,10 @@
         <v>40</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D352" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="E352" s="3" t="n">
         <v>59</v>
@@ -14557,7 +14647,7 @@
         <v>Чорновола В.,просп.  59 Львів</v>
       </c>
       <c r="K352" s="0" t="s">
-        <v>899</v>
+        <v>903</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14568,10 +14658,10 @@
         <v>13</v>
       </c>
       <c r="C353" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D353" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="E353" s="3" t="n">
         <v>57</v>
@@ -14583,14 +14673,14 @@
         <v>1</v>
       </c>
       <c r="I353" s="2" t="s">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c r="J353" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D353,  " ", E353, " ", "Львів")</f>
         <v>Чорновола В.,просп.  57 Львів</v>
       </c>
       <c r="K353" s="0" t="s">
-        <v>901</v>
+        <v>905</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14601,10 +14691,10 @@
         <v>24</v>
       </c>
       <c r="C354" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D354" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="E354" s="3" t="n">
         <v>65</v>
@@ -14616,14 +14706,14 @@
         <v>3</v>
       </c>
       <c r="I354" s="2" t="s">
-        <v>902</v>
+        <v>906</v>
       </c>
       <c r="J354" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D354,  " ", E354, " ", "Львів")</f>
         <v>Чорновола В.,просп.  65 Львів</v>
       </c>
       <c r="K354" s="0" t="s">
-        <v>903</v>
+        <v>907</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14634,13 +14724,13 @@
         <v>40</v>
       </c>
       <c r="C355" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D355" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="E355" s="3" t="s">
-        <v>904</v>
+        <v>908</v>
       </c>
       <c r="G355" s="0" t="n">
         <v>11</v>
@@ -14649,14 +14739,14 @@
         <v>1</v>
       </c>
       <c r="I355" s="2" t="s">
-        <v>905</v>
+        <v>909</v>
       </c>
       <c r="J355" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D355,  " ", E355, " ", "Львів")</f>
         <v>Чорновола В.,просп.   43-а Львів</v>
       </c>
       <c r="K355" s="0" t="s">
-        <v>906</v>
+        <v>910</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14667,10 +14757,10 @@
         <v>13</v>
       </c>
       <c r="C356" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D356" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="E356" s="3" t="n">
         <v>59</v>
@@ -14689,7 +14779,7 @@
         <v>Чорновола В.,просп.  59 Львів</v>
       </c>
       <c r="K356" s="0" t="s">
-        <v>899</v>
+        <v>903</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14703,10 +14793,10 @@
         <v>14</v>
       </c>
       <c r="D357" s="0" t="s">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c r="E357" s="3" t="s">
-        <v>908</v>
+        <v>912</v>
       </c>
       <c r="G357" s="0" t="n">
         <v>2</v>
@@ -14715,14 +14805,14 @@
         <v>1</v>
       </c>
       <c r="I357" s="2" t="s">
-        <v>909</v>
+        <v>913</v>
       </c>
       <c r="J357" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D357,  " ", E357, " ", "Львів")</f>
         <v>Шевченка Т.   358-б Львів</v>
       </c>
       <c r="K357" s="0" t="s">
-        <v>910</v>
+        <v>914</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14733,10 +14823,10 @@
         <v>24</v>
       </c>
       <c r="C358" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D358" s="0" t="s">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c r="E358" s="3"/>
       <c r="G358" s="0" t="n">
@@ -14746,14 +14836,14 @@
         <v>10</v>
       </c>
       <c r="I358" s="2" t="s">
-        <v>912</v>
+        <v>916</v>
       </c>
       <c r="J358" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D358,  " ", E358, " ", "Львів")</f>
         <v>Шевченка Т., просп.   Львів</v>
       </c>
       <c r="K358" s="0" t="s">
-        <v>913</v>
+        <v>917</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14764,10 +14854,10 @@
         <v>40</v>
       </c>
       <c r="C359" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D359" s="0" t="s">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c r="E359" s="3" t="n">
         <v>12</v>
@@ -14779,14 +14869,14 @@
         <v>1</v>
       </c>
       <c r="I359" s="2" t="s">
-        <v>914</v>
+        <v>918</v>
       </c>
       <c r="J359" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D359,  " ", E359, " ", "Львів")</f>
         <v>Шевченка Т., просп.  12 Львів</v>
       </c>
       <c r="K359" s="0" t="s">
-        <v>915</v>
+        <v>919</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14797,10 +14887,10 @@
         <v>40</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D360" s="0" t="s">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c r="E360" s="3" t="n">
         <v>7</v>
@@ -14812,14 +14902,14 @@
         <v>1</v>
       </c>
       <c r="I360" s="2" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
       <c r="J360" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D360,  " ", E360, " ", "Львів")</f>
         <v>Шевченка Т., просп.  7 Львів</v>
       </c>
       <c r="K360" s="0" t="s">
-        <v>917</v>
+        <v>921</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14833,11 +14923,11 @@
         <v>14</v>
       </c>
       <c r="D361" s="0" t="s">
-        <v>918</v>
+        <v>922</v>
       </c>
       <c r="E361" s="3"/>
       <c r="F361" s="0" t="s">
-        <v>919</v>
+        <v>923</v>
       </c>
       <c r="G361" s="0" t="n">
         <v>2</v>
@@ -14846,14 +14936,14 @@
         <v>1</v>
       </c>
       <c r="I361" s="2" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="J361" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D361,  " ", E361, " ", "Львів")</f>
         <v>Шевченка Т.  Львів</v>
       </c>
       <c r="K361" s="0" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14867,7 +14957,7 @@
         <v>14</v>
       </c>
       <c r="D362" s="0" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="E362" s="3"/>
       <c r="G362" s="0" t="n">
@@ -14877,14 +14967,14 @@
         <v>1</v>
       </c>
       <c r="I362" s="2" t="s">
-        <v>923</v>
+        <v>927</v>
       </c>
       <c r="J362" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D362,  " ", E362, " ", "Львів")</f>
         <v>Шевченка Т. – Томашівська   Львів</v>
       </c>
       <c r="K362" s="0" t="s">
-        <v>924</v>
+        <v>928</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14898,7 +14988,7 @@
         <v>14</v>
       </c>
       <c r="D363" s="0" t="s">
-        <v>925</v>
+        <v>929</v>
       </c>
       <c r="E363" s="3" t="n">
         <v>18</v>
@@ -14910,14 +15000,14 @@
         <v>1</v>
       </c>
       <c r="I363" s="2" t="s">
-        <v>926</v>
+        <v>930</v>
       </c>
       <c r="J363" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D363,  " ", E363, " ", "Львів")</f>
         <v>Шептицьких  18 Львів</v>
       </c>
       <c r="K363" s="0" t="s">
-        <v>927</v>
+        <v>931</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14931,7 +15021,7 @@
         <v>14</v>
       </c>
       <c r="D364" s="0" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="E364" s="3" t="n">
         <v>85</v>
@@ -14943,14 +15033,14 @@
         <v>4</v>
       </c>
       <c r="I364" s="2" t="s">
-        <v>929</v>
+        <v>933</v>
       </c>
       <c r="J364" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D364,  " ", E364, " ", "Львів")</f>
         <v>Широка  85 Львів</v>
       </c>
       <c r="K364" s="0" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14964,10 +15054,10 @@
         <v>14</v>
       </c>
       <c r="D365" s="0" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="E365" s="3" t="s">
-        <v>931</v>
+        <v>935</v>
       </c>
       <c r="G365" s="0" t="n">
         <v>29</v>
@@ -14976,14 +15066,14 @@
         <v>3</v>
       </c>
       <c r="I365" s="2" t="s">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="J365" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D365,  " ", E365, " ", "Львів")</f>
         <v>Широка   65-а Львів</v>
       </c>
       <c r="K365" s="0" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14997,7 +15087,7 @@
         <v>14</v>
       </c>
       <c r="D366" s="0" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="E366" s="3" t="n">
         <v>41</v>
@@ -15009,14 +15099,14 @@
         <v>3</v>
       </c>
       <c r="I366" s="2" t="s">
-        <v>934</v>
+        <v>938</v>
       </c>
       <c r="J366" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D366,  " ", E366, " ", "Львів")</f>
         <v>Широка  41 Львів</v>
       </c>
       <c r="K366" s="0" t="s">
-        <v>935</v>
+        <v>939</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15030,10 +15120,10 @@
         <v>14</v>
       </c>
       <c r="D367" s="0" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="E367" s="3" t="s">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c r="G367" s="0" t="n">
         <v>10</v>
@@ -15042,14 +15132,14 @@
         <v>1</v>
       </c>
       <c r="I367" s="2" t="s">
-        <v>937</v>
+        <v>941</v>
       </c>
       <c r="J367" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D367,  " ", E367, " ", "Львів")</f>
         <v>Широка   70-а Львів</v>
       </c>
       <c r="K367" s="0" t="s">
-        <v>938</v>
+        <v>942</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15063,7 +15153,7 @@
         <v>14</v>
       </c>
       <c r="D368" s="0" t="s">
-        <v>939</v>
+        <v>943</v>
       </c>
       <c r="E368" s="3"/>
       <c r="G368" s="0" t="n">
@@ -15073,14 +15163,14 @@
         <v>3</v>
       </c>
       <c r="I368" s="2" t="s">
-        <v>940</v>
+        <v>944</v>
       </c>
       <c r="J368" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D368,  " ", E368, " ", "Львів")</f>
         <v>Шолом-Алейхема Ш.   Львів</v>
       </c>
       <c r="K368" s="0" t="s">
-        <v>941</v>
+        <v>945</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15094,7 +15184,7 @@
         <v>14</v>
       </c>
       <c r="D369" s="0" t="s">
-        <v>942</v>
+        <v>946</v>
       </c>
       <c r="E369" s="3"/>
       <c r="G369" s="0" t="n">
@@ -15104,14 +15194,14 @@
         <v>3</v>
       </c>
       <c r="I369" s="2" t="s">
-        <v>943</v>
+        <v>947</v>
       </c>
       <c r="J369" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D369,  " ", E369, " ", "Львів")</f>
         <v>Шпитальна   Львів</v>
       </c>
       <c r="K369" s="0" t="s">
-        <v>944</v>
+        <v>948</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15125,7 +15215,7 @@
         <v>14</v>
       </c>
       <c r="D370" s="0" t="s">
-        <v>942</v>
+        <v>946</v>
       </c>
       <c r="E370" s="3" t="n">
         <v>1</v>
@@ -15137,14 +15227,14 @@
         <v>3</v>
       </c>
       <c r="I370" s="2" t="s">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c r="J370" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D370,  " ", E370, " ", "Львів")</f>
         <v>Шпитальна  1 Львів</v>
       </c>
       <c r="K370" s="0" t="s">
-        <v>946</v>
+        <v>950</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15158,7 +15248,7 @@
         <v>14</v>
       </c>
       <c r="D371" s="0" t="s">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c r="E371" s="3"/>
       <c r="G371" s="0" t="n">
@@ -15168,14 +15258,14 @@
         <v>1</v>
       </c>
       <c r="I371" s="2" t="s">
-        <v>948</v>
+        <v>952</v>
       </c>
       <c r="J371" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D371,  " ", E371, " ", "Львів")</f>
         <v>Шухевича В.   Львів</v>
       </c>
       <c r="K371" s="0" t="s">
-        <v>949</v>
+        <v>953</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15189,7 +15279,7 @@
         <v>14</v>
       </c>
       <c r="D372" s="0" t="s">
-        <v>950</v>
+        <v>954</v>
       </c>
       <c r="E372" s="3"/>
       <c r="G372" s="0" t="n">
@@ -15199,14 +15289,14 @@
         <v>1</v>
       </c>
       <c r="I372" s="2" t="s">
-        <v>951</v>
+        <v>955</v>
       </c>
       <c r="J372" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D372,  " ", E372, " ", "Львів")</f>
         <v>Любінська - Д.Яворницького   Львів</v>
       </c>
       <c r="K372" s="0" t="s">
-        <v>952</v>
+        <v>956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>